<commit_message>
updated: data source, data structure added: basic plot, basic  moving average
</commit_message>
<xml_diff>
--- a/data/retail.xlsx
+++ b/data/retail.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Le Minh Pham Hoang\PycharmProjects\Demand-Forecasting\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all_items" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,13 @@
     <sheet name="tennis_short" sheetId="12" r:id="rId4"/>
     <sheet name="tennis_racket" sheetId="11" r:id="rId5"/>
     <sheet name="socks" sheetId="10" r:id="rId6"/>
-    <sheet name="hard_tennis_ball_pack" sheetId="8" r:id="rId7"/>
-    <sheet name="clay_tennis_shoes" sheetId="7" r:id="rId8"/>
-    <sheet name="clay_tennis_ball_pack" sheetId="6" r:id="rId9"/>
-    <sheet name="all_surface_tennis_shoes" sheetId="5" r:id="rId10"/>
-    <sheet name="all_sports_gear" sheetId="3" r:id="rId11"/>
+    <sheet name="novak_racket" sheetId="9" r:id="rId7"/>
+    <sheet name="hard_tennis_ball_pack" sheetId="8" r:id="rId8"/>
+    <sheet name="clay_tennis_shoes" sheetId="7" r:id="rId9"/>
+    <sheet name="clay_tennis_ball_pack" sheetId="6" r:id="rId10"/>
+    <sheet name="all_surface_tennis_shoes" sheetId="5" r:id="rId11"/>
     <sheet name="all_surface_tennis_ball_pack" sheetId="4" r:id="rId12"/>
-    <sheet name="novak_racket" sheetId="9" r:id="rId13"/>
+    <sheet name="all_sports_gear" sheetId="3" r:id="rId13"/>
     <sheet name="all_material" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -181,9 +181,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,19 +487,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.125" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -511,7 +508,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -522,7 +519,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -533,7 +530,7 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -544,7 +541,7 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -555,7 +552,7 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -566,7 +563,7 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -577,7 +574,7 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -588,7 +585,7 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -599,7 +596,7 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -610,7 +607,7 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -621,7 +618,7 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -632,7 +629,7 @@
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -643,7 +640,7 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -654,7 +651,7 @@
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -665,7 +662,7 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -676,7 +673,7 @@
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -687,7 +684,7 @@
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -698,7 +695,7 @@
       <c r="A19" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -709,7 +706,7 @@
       <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -720,7 +717,7 @@
       <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -731,7 +728,7 @@
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -742,7 +739,7 @@
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -753,7 +750,7 @@
       <c r="A24" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -762,7 +759,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -771,184 +767,181 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -957,9 +950,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -968,9 +961,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -979,9 +972,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -990,9 +983,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1001,9 +994,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -1012,9 +1005,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1023,9 +1016,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -1034,9 +1027,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -1053,184 +1046,181 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>44</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>146</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>145</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>141</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1239,9 +1229,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -1250,9 +1240,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -1261,9 +1251,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -1272,9 +1262,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1283,9 +1273,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -1294,9 +1284,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1305,9 +1295,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -1316,9 +1306,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -1335,19 +1325,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -1358,7 +1345,7 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -1369,7 +1356,7 @@
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -1380,7 +1367,7 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -1391,7 +1378,7 @@
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -1402,7 +1389,7 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -1413,7 +1400,7 @@
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -1424,7 +1411,7 @@
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -1435,7 +1422,7 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -1446,7 +1433,7 @@
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -1457,7 +1444,7 @@
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -1468,7 +1455,7 @@
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -1479,7 +1466,7 @@
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -1490,7 +1477,7 @@
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -1501,7 +1488,7 @@
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -1512,7 +1499,7 @@
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1523,7 +1510,7 @@
       <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -1534,7 +1521,7 @@
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -1545,7 +1532,7 @@
       <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -1556,7 +1543,7 @@
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1567,7 +1554,7 @@
       <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -1578,7 +1565,7 @@
       <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1589,7 +1576,7 @@
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -1600,7 +1587,7 @@
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -1617,184 +1604,181 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>19</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -1803,9 +1787,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -1814,9 +1798,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -1825,9 +1809,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -1836,9 +1820,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -1847,9 +1831,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -1858,9 +1842,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -1869,9 +1853,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -1880,9 +1864,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -1899,19 +1883,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -1922,7 +1903,7 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -1933,7 +1914,7 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -1944,7 +1925,7 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -1955,7 +1936,7 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -1966,7 +1947,7 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -1977,7 +1958,7 @@
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -1988,7 +1969,7 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -1999,7 +1980,7 @@
       <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -2010,7 +1991,7 @@
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -2021,7 +2002,7 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -2032,7 +2013,7 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -2043,7 +2024,7 @@
       <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -2054,7 +2035,7 @@
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -2065,7 +2046,7 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -2076,7 +2057,7 @@
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -2087,7 +2068,7 @@
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -2098,7 +2079,7 @@
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -2109,7 +2090,7 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -2120,7 +2101,7 @@
       <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -2131,7 +2112,7 @@
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -2142,7 +2123,7 @@
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -2153,7 +2134,7 @@
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -2164,7 +2145,7 @@
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -2180,21 +2161,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -2205,7 +2182,7 @@
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -2216,7 +2193,7 @@
       <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -2227,7 +2204,7 @@
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -2238,7 +2215,7 @@
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -2249,7 +2226,7 @@
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -2260,7 +2237,7 @@
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -2271,7 +2248,7 @@
       <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -2282,7 +2259,7 @@
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -2293,7 +2270,7 @@
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -2304,7 +2281,7 @@
       <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -2315,7 +2292,7 @@
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -2326,7 +2303,7 @@
       <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -2337,7 +2314,7 @@
       <c r="A14" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -2348,7 +2325,7 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -2359,7 +2336,7 @@
       <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -2370,7 +2347,7 @@
       <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -2381,7 +2358,7 @@
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -2392,7 +2369,7 @@
       <c r="A19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -2403,7 +2380,7 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -2414,7 +2391,7 @@
       <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -2425,7 +2402,7 @@
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -2436,7 +2413,7 @@
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -2447,7 +2424,7 @@
       <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -2464,19 +2441,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -2487,7 +2461,7 @@
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -2498,7 +2472,7 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -2509,7 +2483,7 @@
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -2520,7 +2494,7 @@
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -2531,7 +2505,7 @@
       <c r="A6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -2542,7 +2516,7 @@
       <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -2553,7 +2527,7 @@
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -2564,7 +2538,7 @@
       <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -2575,7 +2549,7 @@
       <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -2586,7 +2560,7 @@
       <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -2597,7 +2571,7 @@
       <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -2608,7 +2582,7 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -2619,7 +2593,7 @@
       <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -2630,7 +2604,7 @@
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -2641,7 +2615,7 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -2652,7 +2626,7 @@
       <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -2663,7 +2637,7 @@
       <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -2674,7 +2648,7 @@
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -2685,7 +2659,7 @@
       <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -2696,7 +2670,7 @@
       <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -2707,7 +2681,7 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -2718,7 +2692,7 @@
       <c r="A23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -2729,7 +2703,7 @@
       <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -2746,19 +2720,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -2769,7 +2740,7 @@
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -2780,7 +2751,7 @@
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -2791,7 +2762,7 @@
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -2802,7 +2773,7 @@
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -2813,7 +2784,7 @@
       <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -2824,7 +2795,7 @@
       <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -2835,7 +2806,7 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -2846,7 +2817,7 @@
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -2857,7 +2828,7 @@
       <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -2868,7 +2839,7 @@
       <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -2879,7 +2850,7 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -2890,7 +2861,7 @@
       <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -2901,7 +2872,7 @@
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -2912,7 +2883,7 @@
       <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -2923,7 +2894,7 @@
       <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -2934,7 +2905,7 @@
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -2945,7 +2916,7 @@
       <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -2956,7 +2927,7 @@
       <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -2967,7 +2938,7 @@
       <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -2978,7 +2949,7 @@
       <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -2989,7 +2960,7 @@
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -3000,7 +2971,7 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -3011,7 +2982,7 @@
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -3028,19 +2999,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -3051,7 +3019,7 @@
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -3062,7 +3030,7 @@
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -3073,7 +3041,7 @@
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -3084,7 +3052,7 @@
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -3095,7 +3063,7 @@
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -3106,7 +3074,7 @@
       <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -3117,7 +3085,7 @@
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -3128,7 +3096,7 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -3139,7 +3107,7 @@
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -3150,7 +3118,7 @@
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -3161,7 +3129,7 @@
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -3172,7 +3140,7 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -3183,7 +3151,7 @@
       <c r="A14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -3194,7 +3162,7 @@
       <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -3205,7 +3173,7 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -3216,7 +3184,7 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -3227,7 +3195,7 @@
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -3238,7 +3206,7 @@
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -3249,7 +3217,7 @@
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -3260,7 +3228,7 @@
       <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -3271,7 +3239,7 @@
       <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -3282,7 +3250,7 @@
       <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -3293,7 +3261,7 @@
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -3310,19 +3278,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -3333,7 +3298,7 @@
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
@@ -3344,7 +3309,7 @@
       <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -3355,7 +3320,7 @@
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -3366,7 +3331,7 @@
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -3377,7 +3342,7 @@
       <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -3388,7 +3353,7 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -3399,7 +3364,7 @@
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -3410,7 +3375,7 @@
       <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -3421,7 +3386,7 @@
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -3432,7 +3397,7 @@
       <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -3443,7 +3408,7 @@
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
@@ -3454,7 +3419,7 @@
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
@@ -3465,7 +3430,7 @@
       <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
@@ -3476,7 +3441,7 @@
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
@@ -3487,7 +3452,7 @@
       <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -3498,7 +3463,7 @@
       <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -3509,7 +3474,7 @@
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -3520,7 +3485,7 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -3531,7 +3496,7 @@
       <c r="A20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -3542,7 +3507,7 @@
       <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -3553,7 +3518,7 @@
       <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -3564,7 +3529,7 @@
       <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -3575,7 +3540,7 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -3592,184 +3557,181 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
         <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -3778,9 +3740,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -3789,9 +3751,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -3800,9 +3762,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -3811,9 +3773,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -3822,9 +3784,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -3833,9 +3795,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -3844,9 +3806,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -3855,9 +3817,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -3874,19 +3836,16 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="9" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
@@ -3895,20 +3854,20 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
@@ -3917,141 +3876,141 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -4060,9 +4019,9 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17">
@@ -4071,9 +4030,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18">
@@ -4082,9 +4041,9 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19">
@@ -4093,9 +4052,9 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20">
@@ -4104,9 +4063,9 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21">
@@ -4115,9 +4074,9 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22">
@@ -4126,9 +4085,9 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23">
@@ -4137,9 +4096,9 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24">
@@ -4153,185 +4112,182 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -4340,9 +4296,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -4351,9 +4307,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -4362,9 +4318,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -4373,9 +4329,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -4384,9 +4340,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -4394,11 +4350,10 @@
       <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -4407,9 +4362,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -4418,9 +4373,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>

</xml_diff>